<commit_message>
Additional fixes to bring S1 and Figure 2 into complete agreement
</commit_message>
<xml_diff>
--- a/plos-revisions/prep/figure_prep/fig2/heatmap.xlsx
+++ b/plos-revisions/prep/figure_prep/fig2/heatmap.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="593" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="593" uniqueCount="224">
   <si>
     <t>sample</t>
   </si>
@@ -693,6 +693,9 @@
   </si>
   <si>
     <t>F72A</t>
+  </si>
+  <si>
+    <t>M323G</t>
   </si>
 </sst>
 </file>
@@ -829,8 +832,14 @@
       </diagonal>
     </border>
   </borders>
-  <cellStyleXfs count="57">
+  <cellStyleXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -925,7 +934,7 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="57">
+  <cellStyles count="63">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -954,6 +963,9 @@
     <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -982,9 +994,60 @@
     <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="6">
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <strike val="0"/>
@@ -1607,11 +1670,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2124893720"/>
-        <c:axId val="2124896680"/>
+        <c:axId val="2091290120"/>
+        <c:axId val="2091287160"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2124893720"/>
+        <c:axId val="2091290120"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -1622,12 +1685,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2124896680"/>
+        <c:crossAx val="2091287160"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2124896680"/>
+        <c:axId val="2091287160"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -1639,7 +1702,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2124893720"/>
+        <c:crossAx val="2091290120"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -8174,7 +8237,7 @@
   <dimension ref="B1:AR113"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A80" zoomScale="15" zoomScaleNormal="15" zoomScalePageLayoutView="15" workbookViewId="0">
-      <selection activeCell="AL98" sqref="AL98"/>
+      <selection activeCell="AD8" sqref="AD8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="180" customHeight="1" x14ac:dyDescent="0"/>
@@ -8569,7 +8632,9 @@
       </c>
       <c r="C21" s="8"/>
       <c r="D21" s="8"/>
-      <c r="E21" s="8"/>
+      <c r="E21" s="10">
+        <v>-5</v>
+      </c>
       <c r="F21" s="10"/>
       <c r="G21" s="14" t="s">
         <v>133</v>
@@ -9174,12 +9239,8 @@
       <c r="B55" s="11">
         <v>0.11</v>
       </c>
-      <c r="C55" s="6">
-        <v>-1.1568715528486477</v>
-      </c>
-      <c r="D55" s="6">
-        <v>-0.29251414474145143</v>
-      </c>
+      <c r="C55" s="8"/>
+      <c r="D55" s="8"/>
       <c r="E55" s="6">
         <v>-1.4493851744040676</v>
       </c>
@@ -9401,7 +9462,7 @@
         <v>-1.3304152914216902</v>
       </c>
       <c r="G68" s="14" t="s">
-        <v>162</v>
+        <v>223</v>
       </c>
       <c r="M68" s="21"/>
     </row>
@@ -9814,17 +9875,11 @@
     </row>
     <row r="94" spans="2:37" ht="180" customHeight="1">
       <c r="B94" s="11">
-        <v>0.13</v>
-      </c>
-      <c r="C94" s="6">
-        <v>-1.8895474136766004</v>
-      </c>
-      <c r="D94" s="6">
-        <v>-0.16957742772938156</v>
-      </c>
-      <c r="E94" s="6">
-        <v>-2.0591319943983213</v>
-      </c>
+        <v>0.1</v>
+      </c>
+      <c r="C94" s="8"/>
+      <c r="D94" s="8"/>
+      <c r="E94" s="8"/>
       <c r="G94" s="14" t="s">
         <v>208</v>
       </c>
@@ -9986,8 +10041,8 @@
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
-  <conditionalFormatting sqref="C2:E1048576">
-    <cfRule type="colorScale" priority="8">
+  <conditionalFormatting sqref="C95:E1048576 C2:E93">
+    <cfRule type="colorScale" priority="11">
       <colorScale>
         <cfvo type="num" val="-5"/>
         <cfvo type="num" val="0"/>
@@ -9999,7 +10054,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AQ3:AQ9">
-    <cfRule type="colorScale" priority="7">
+    <cfRule type="colorScale" priority="10">
       <colorScale>
         <cfvo type="num" val="-5"/>
         <cfvo type="num" val="0"/>
@@ -10010,12 +10065,34 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="between">
+  <conditionalFormatting sqref="B1:B93 B95:B1048576">
+    <cfRule type="cellIs" dxfId="5" priority="4" operator="between">
       <formula>0.11</formula>
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="4" operator="between">
+    <cfRule type="cellIs" dxfId="4" priority="7" operator="between">
+      <formula>0</formula>
+      <formula>0.1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C94:E94">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="num" val="-5"/>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color rgb="FF00305B"/>
+        <color theme="0" tint="-4.9989318521683403E-2"/>
+        <color rgb="FFCCA11B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B94">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="between">
+      <formula>0.11</formula>
+      <formula>2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="between">
       <formula>0</formula>
       <formula>0.1</formula>
     </cfRule>

</xml_diff>